<commit_message>
Deleted files, deleted variables in script and updated the code accordingly
</commit_message>
<xml_diff>
--- a/Codebook_RMED901_exam_group4.xlsx
+++ b/Codebook_RMED901_exam_group4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofbergen-my.sharepoint.com/personal/bente_skottvoll_uib_no/Documents/2022-PhD/Kurs/2023 09 RMED901/RMED901_Group4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{80A817C1-BFB2-4208-8780-7912B9D6EF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D77C3472-8CF7-4125-BD27-AC6B67B7F544}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{80A817C1-BFB2-4208-8780-7912B9D6EF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57DFB3F0-5D74-4DC2-AE59-FBF692D17AD4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t xml:space="preserve">variable </t>
   </si>
@@ -104,9 +104,6 @@
     <t xml:space="preserve">streptomycin resistance after 6 months of therapy, measured on a 0-100+ scale, categorized into 3 levels - sensitive, moderate, and resistant </t>
   </si>
   <si>
-    <t xml:space="preserve">6m_radiologic </t>
-  </si>
-  <si>
     <t xml:space="preserve">Likert score rating of radiologic response on chest x-ray at 6 months </t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>1= Death, 2= Considerable deterioration, 3= Moderate deterioration, 4= No change, 5= Moderate improvement, 6= Considerable improvement</t>
   </si>
   <si>
-    <t>Gender_numeric</t>
-  </si>
-  <si>
     <t>task line 50</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>task line</t>
   </si>
   <si>
-    <t>use in plotting</t>
-  </si>
-  <si>
     <t>encoding</t>
   </si>
   <si>
@@ -294,6 +285,21 @@
   </si>
   <si>
     <t>no or yes</t>
+  </si>
+  <si>
+    <t>gender_numeric</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X6m_radiologic </t>
+  </si>
+  <si>
+    <t>renamed from 6m_radiologic and deleted day 6</t>
+  </si>
+  <si>
+    <t>new, deleted day 6</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -673,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BE8A21-2C37-4DF0-BCC6-103D7F0C1190}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,19 +696,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -717,10 +719,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -728,16 +727,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -745,16 +744,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -768,7 +764,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -782,7 +778,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -790,16 +786,13 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -807,10 +800,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -818,36 +811,33 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -855,10 +845,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -866,33 +856,36 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -903,27 +896,27 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -931,10 +924,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -942,16 +935,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -969,191 +962,236 @@
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>86</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" t="s">
-        <v>25</v>
+      <c r="G26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
         <v>32</v>
       </c>
-      <c r="F29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
udated the codebook with marking the deleted columns.
</commit_message>
<xml_diff>
--- a/Codebook_RMED901_exam_group4.xlsx
+++ b/Codebook_RMED901_exam_group4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofbergen-my.sharepoint.com/personal/bente_skottvoll_uib_no/Documents/2022-PhD/Kurs/2023 09 RMED901/RMED901_Group4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieskildrasmussen/Documents/Kurs/RMED901/RMED901_Group4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="8_{80A817C1-BFB2-4208-8780-7912B9D6EF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57DFB3F0-5D74-4DC2-AE59-FBF692D17AD4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D8F7C7-A202-4F4A-84E6-7CB8300E9602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t xml:space="preserve">variable </t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>new, deleted day 6</t>
+  </si>
+  <si>
+    <t>deleted day 8</t>
+  </si>
+  <si>
+    <t>new, deleted day 8</t>
   </si>
 </sst>
 </file>
@@ -678,17 +684,17 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="50.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +717,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -722,24 +728,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3">
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -753,7 +762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -767,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -781,7 +790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -795,7 +804,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -809,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -826,7 +835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -840,7 +849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -854,24 +863,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12">
+      <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -888,7 +897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -902,24 +911,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15">
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -933,24 +942,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17">
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -965,7 +974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -982,35 +991,35 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20">
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E21" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21">
+      <c r="E21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1041,58 +1050,64 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G25">
+      <c r="E25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G26">
+      <c r="E26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1112,7 +1127,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1129,7 +1144,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1149,47 +1164,47 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Deleted temporary placed text in cells
</commit_message>
<xml_diff>
--- a/Codebook_RMED901_exam_group4.xlsx
+++ b/Codebook_RMED901_exam_group4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieskildrasmussen/Documents/Kurs/RMED901/RMED901_Group4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fec011\OneDrive - University of Bergen\2022-PhD\Kurs\2023 09 RMED901\RMED901_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D8F7C7-A202-4F4A-84E6-7CB8300E9602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A653E04F-B2C4-4E6C-976F-43FA24A59EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
   <si>
     <t xml:space="preserve">variable </t>
   </si>
@@ -681,20 +681,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BE8A21-2C37-4DF0-BCC6-103D7F0C1190}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="50.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="50.77734375" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +717,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -728,7 +728,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -762,7 +762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -790,7 +790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -804,7 +804,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -818,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -835,7 +835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -849,7 +849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -863,7 +863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -880,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -897,7 +897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -911,7 +911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -942,7 +942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -974,7 +974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -991,7 +991,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1162,51 +1162,6 @@
       </c>
       <c r="F29" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text cleaning, deleted sections with log text chunks in Exam report.rmd, updated codebook with day 8 variable and formatted README
</commit_message>
<xml_diff>
--- a/Codebook_RMED901_exam_group4.xlsx
+++ b/Codebook_RMED901_exam_group4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fec011\OneDrive - University of Bergen\2022-PhD\Kurs\2023 09 RMED901\RMED901_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A653E04F-B2C4-4E6C-976F-43FA24A59EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC9BEFA-A49A-44EB-894E-607D0FEF5383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9EF4F3A5-D269-4F2B-884F-B6CEB8D7837F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t xml:space="preserve">variable </t>
   </si>
@@ -306,6 +306,21 @@
   </si>
   <si>
     <t>new, deleted day 8</t>
+  </si>
+  <si>
+    <t>arm_numeric</t>
+  </si>
+  <si>
+    <t>assigned treatment arm, created from variable arm to be numeric</t>
+  </si>
+  <si>
+    <t>Control = 0, Intervention by Streptomycin = 1</t>
+  </si>
+  <si>
+    <t>numric</t>
+  </si>
+  <si>
+    <t>new, day 8</t>
   </si>
 </sst>
 </file>
@@ -681,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3BE8A21-2C37-4DF0-BCC6-103D7F0C1190}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,6 +1179,26 @@
         <v>46</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G29" xr:uid="{F3BE8A21-2C37-4DF0-BCC6-103D7F0C1190}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>